<commit_message>
new cost estimate commit
</commit_message>
<xml_diff>
--- a/Schedule Management .xlsx
+++ b/Schedule Management .xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538360\Documents\github\GDP-1-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538336\Desktop\GDP-1-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1688D3-A17B-4E37-9E8D-2BB2C647CD4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Work Breakdown Structure Categories</t>
   </si>
@@ -86,58 +85,40 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Responsible</t>
-  </si>
-  <si>
     <t>Estimated Hours per person</t>
   </si>
   <si>
-    <t>Sumana Reddy</t>
-  </si>
-  <si>
-    <t>Pooja</t>
-  </si>
-  <si>
-    <t>Vikas</t>
-  </si>
-  <si>
-    <t>Sumanth</t>
-  </si>
-  <si>
-    <t>Rajashekar</t>
-  </si>
-  <si>
-    <t>Rohith</t>
-  </si>
-  <si>
     <t>Total Est.Hours</t>
   </si>
   <si>
     <t>11/31/2020</t>
   </si>
   <si>
-    <t>Team</t>
-  </si>
-  <si>
-    <t>Sumana</t>
-  </si>
-  <si>
-    <t>pooja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vikas </t>
-  </si>
-  <si>
-    <t>Rohit</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                                                                                                    Schedule Management - Team : 01</t>
+  </si>
+  <si>
+    <t>Developer 1</t>
+  </si>
+  <si>
+    <t>Developer 2</t>
+  </si>
+  <si>
+    <t>Developer 3</t>
+  </si>
+  <si>
+    <t>Developer 4</t>
+  </si>
+  <si>
+    <t>Developer 5</t>
+  </si>
+  <si>
+    <t>Developer 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,30 +468,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" customWidth="1"/>
-    <col min="9" max="9" width="9.453125" customWidth="1"/>
-    <col min="11" max="11" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,44 +507,40 @@
       <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -570,33 +550,30 @@
       <c r="C7" s="6">
         <v>44066</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
+      <c r="D7" s="2">
+        <v>2</v>
       </c>
       <c r="E7" s="2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F7" s="2">
         <v>1.5</v>
       </c>
       <c r="G7" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="2">
-        <v>2</v>
-      </c>
-      <c r="K7" s="2">
-        <f>E7+F7+G7+H7+I7+J7</f>
+        <f>D7+E7+F7+G7+H7+I7</f>
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -606,33 +583,30 @@
       <c r="C8" s="6">
         <v>44067</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
+      <c r="D8" s="2">
+        <v>1</v>
       </c>
       <c r="E8" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F8" s="2">
         <v>1.5</v>
       </c>
       <c r="G8" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H8" s="2">
         <v>2</v>
       </c>
       <c r="I8" s="2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J8" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="K8" s="2">
-        <f>E8+F8+G8+H8+I8+J8</f>
+        <f>D8+E8+F8+G8+H8+I8</f>
         <v>9.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -640,35 +614,32 @@
         <v>44068</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.5</v>
       </c>
       <c r="E9" s="2">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="F9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" s="2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="H9" s="2">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="I9" s="2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2">
-        <f>E9+F9+G9+H9+I9+J9</f>
+        <f>D9+E9+F9+G9+H9+I9</f>
         <v>11.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -678,23 +649,20 @@
       <c r="C10" s="6">
         <v>44089</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
         <v>6</v>
       </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2">
-        <f>F10</f>
+      <c r="J10" s="2">
+        <f>E10</f>
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -704,31 +672,28 @@
       <c r="C11" s="6">
         <v>44119</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>27</v>
+      <c r="D11" s="2">
+        <v>1.5</v>
       </c>
       <c r="E11" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2">
         <v>2.5</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
+        <v>1.5</v>
+      </c>
       <c r="I11" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="J11" s="2">
-        <v>2</v>
-      </c>
-      <c r="K11" s="2">
-        <f>E11+F11+G11+H11+I11+J11</f>
+        <f>D11+E11+F11+G11+H11+I11</f>
         <v>9.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -738,23 +703,20 @@
       <c r="C12" s="5">
         <v>44139</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
+      <c r="F12" s="2">
         <v>5.5</v>
       </c>
+      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2">
-        <f>G12</f>
+      <c r="J12" s="2">
+        <f>F12</f>
         <v>5.5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -762,25 +724,22 @@
         <v>44140</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2">
+      <c r="H13" s="2">
         <v>7</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2">
-        <f>I13</f>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
+        <f>H13</f>
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -790,33 +749,30 @@
       <c r="C14" s="5">
         <v>44285</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>27</v>
+      <c r="D14" s="2">
+        <v>1</v>
       </c>
       <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="I14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="2">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2">
-        <v>3</v>
-      </c>
-      <c r="H14" s="2">
-        <v>2</v>
-      </c>
-      <c r="I14" s="2">
-        <v>1.5</v>
-      </c>
       <c r="J14" s="2">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2">
-        <f>E14+F14+G14+H14+I14+J14</f>
+        <f>D14+E14+F14+G14+H14+I14</f>
         <v>10.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -826,33 +782,30 @@
       <c r="C15" s="5">
         <v>44232</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>27</v>
+      <c r="D15" s="2">
+        <v>2</v>
       </c>
       <c r="E15" s="2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F15" s="2">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="G15" s="2">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="H15" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="I15" s="2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J15" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="K15" s="2">
-        <f>E15+F15+G15+H15+I15+J15</f>
+        <f>D15+E15+F15+G15+H15+I15</f>
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -862,23 +815,20 @@
       <c r="C16" s="5">
         <v>44255</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="D16" s="2">
         <v>5</v>
       </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2">
-        <f>E16</f>
+      <c r="J16" s="2">
+        <f>D16</f>
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -888,23 +838,20 @@
       <c r="C17" s="5">
         <v>44285</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2">
+      <c r="G17" s="2">
         <v>6</v>
       </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2">
-        <f>H17</f>
+      <c r="J17" s="2">
+        <f>G17</f>
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -914,33 +861,30 @@
       <c r="C18" s="5">
         <v>44303</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>27</v>
+      <c r="D18" s="2">
+        <v>1</v>
       </c>
       <c r="E18" s="2">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="F18" s="2">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="G18" s="2">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="H18" s="2">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="I18" s="2">
         <v>1.5</v>
       </c>
       <c r="J18" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="K18" s="2">
-        <f>E18+F18+G18+H18+I18+J18</f>
+        <f>D18+E18+F18+G18+H18+I18</f>
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -950,55 +894,51 @@
       <c r="C19" s="5">
         <v>44317</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="I19" s="2">
+        <v>6.5</v>
+      </c>
       <c r="J19" s="2">
+        <f>I19</f>
         <v>6.5</v>
       </c>
-      <c r="K19" s="2">
-        <f>J19</f>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <f>D7+D8+D9+D11+D14+D15+D16+D18</f>
+        <v>15</v>
+      </c>
       <c r="E20" s="2">
-        <f>E7+E8+E9+E11+E14+E15+E16+E18</f>
-        <v>15</v>
+        <f>E7+E8+E9+E10+E11+E14+E15+E18</f>
+        <v>20</v>
       </c>
       <c r="F20" s="2">
-        <f>F7+F8+F9+F10+F11+F14+F15+F18</f>
+        <f>F7+F8+F9+F11+F12+F14+F15+F18</f>
         <v>20</v>
       </c>
       <c r="G20" s="2">
-        <f>G7+G8+G9+G11+G12+G14+G15+G18</f>
+        <f>G7+G8+G9+G14+G15+G17+G18</f>
         <v>20</v>
       </c>
       <c r="H20" s="2">
-        <f>H7+H8+H9+H14+H15+H17+H18</f>
-        <v>20</v>
+        <f>H7+H8+H9+H11+H13+H14+H15+H18</f>
+        <v>18</v>
       </c>
       <c r="I20" s="2">
-        <f>I7+I8+I9+I11+I13+I14+I15+I18</f>
-        <v>18</v>
+        <f>I7+I8+I9+I11+I14+I15+I18+I19</f>
+        <v>17</v>
       </c>
       <c r="J20" s="2">
-        <f>J7+J8+J9+J11+J14+J15+J18+J19</f>
-        <v>17</v>
-      </c>
-      <c r="K20" s="2">
-        <f>K7+K8+K9+K10+K11+K12+K13+K14+K15+K16+K17+K18+K19</f>
+        <f>J7+J8+J9+J10+J11+J12+J13+J14+J15+J16+J17+J18+J19</f>
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Readme file is updated as per client instructions. User may be male or female so it is changed as he/she
</commit_message>
<xml_diff>
--- a/Schedule Management .xlsx
+++ b/Schedule Management .xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538360\Documents\github\GDP-1-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057F082D-B6AD-447A-BC53-0E80EAF4BDCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F63B4A-681E-4AEC-8400-AA237FF254C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -173,6 +174,9 @@
       </rPr>
       <t xml:space="preserve"> in hours</t>
     </r>
+  </si>
+  <si>
+    <t>Sheet</t>
   </si>
 </sst>
 </file>
@@ -870,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D285C303-1EFA-4ED6-8202-1217355840E9}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -1724,4 +1728,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097D92D-BD67-4257-A500-74BACB5D2513}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added duration in hours in table.
</commit_message>
<xml_diff>
--- a/Schedule Management .xlsx
+++ b/Schedule Management .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538360\Documents\github\GDP-1-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A8AC2-2B09-454F-8D10-3769BFDD6363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0800A69C-BAE7-4308-B86B-840AFC5D5C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -810,7 +810,7 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -890,7 +890,8 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="6">
-        <v>1</v>
+        <f>D7+D8+D9+D10+D11+D12+D13+D14</f>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -904,7 +905,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="14">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -918,7 +919,7 @@
         <v>40</v>
       </c>
       <c r="D8" s="14">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -932,7 +933,7 @@
         <v>40</v>
       </c>
       <c r="D9" s="14">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.35">
@@ -946,7 +947,7 @@
         <v>40</v>
       </c>
       <c r="D10" s="14">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -960,7 +961,7 @@
         <v>40</v>
       </c>
       <c r="D11" s="14">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -974,7 +975,7 @@
         <v>41</v>
       </c>
       <c r="D12" s="14">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -987,7 +988,9 @@
       <c r="C13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="24"/>
+      <c r="D13" s="24">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="9">
@@ -1000,7 +1003,7 @@
         <v>40</v>
       </c>
       <c r="D14" s="15">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.35">
@@ -1012,7 +1015,8 @@
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="7">
-        <v>1</v>
+        <f>D16+D17+D18+D19+D20</f>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -1026,7 +1030,7 @@
         <v>39</v>
       </c>
       <c r="D16" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1040,7 +1044,7 @@
         <v>39</v>
       </c>
       <c r="D17" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -1054,7 +1058,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -1067,7 +1071,9 @@
       <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="24"/>
+      <c r="D19" s="24">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="9">
@@ -1080,7 +1086,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="15">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
@@ -1092,7 +1098,8 @@
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="7">
-        <v>1</v>
+        <f>D22+D23+D24+D25+D26</f>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1106,7 +1113,7 @@
         <v>39</v>
       </c>
       <c r="D22" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -1120,7 +1127,7 @@
         <v>39</v>
       </c>
       <c r="D23" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1134,7 +1141,7 @@
         <v>39</v>
       </c>
       <c r="D24" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -1147,8 +1154,8 @@
       <c r="C25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="14">
-        <v>1</v>
+      <c r="D25" s="24">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1161,8 +1168,8 @@
       <c r="C26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="14">
-        <v>1</v>
+      <c r="D26" s="15">
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
@@ -1174,7 +1181,8 @@
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="7">
-        <v>1</v>
+        <f>D28+D29+D30+D31+D32</f>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1188,7 +1196,7 @@
         <v>39</v>
       </c>
       <c r="D28" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1202,7 +1210,7 @@
         <v>39</v>
       </c>
       <c r="D29" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1216,7 +1224,7 @@
         <v>39</v>
       </c>
       <c r="D30" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1229,8 +1237,8 @@
       <c r="C31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="15">
-        <v>1</v>
+      <c r="D31" s="24">
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1244,7 +1252,7 @@
         <v>39</v>
       </c>
       <c r="D32" s="15">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -1256,7 +1264,8 @@
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="7">
-        <v>1</v>
+        <f>D34+D35+D36+D37+D38</f>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1270,7 +1279,7 @@
         <v>39</v>
       </c>
       <c r="D34" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1284,7 +1293,7 @@
         <v>39</v>
       </c>
       <c r="D35" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1298,7 +1307,7 @@
         <v>39</v>
       </c>
       <c r="D36" s="14">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1311,8 +1320,8 @@
       <c r="C37" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="15">
-        <v>1</v>
+      <c r="D37" s="24">
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1326,7 +1335,7 @@
         <v>39</v>
       </c>
       <c r="D38" s="15">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Changes made in schedule
</commit_message>
<xml_diff>
--- a/Schedule Management .xlsx
+++ b/Schedule Management .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538360\Documents\github\GDP-1-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0800A69C-BAE7-4308-B86B-840AFC5D5C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320EAF8C-C133-4646-8453-BD19CDA0E8ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,79 +444,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -524,6 +473,60 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -809,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D285C303-1EFA-4ED6-8202-1217355840E9}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -823,43 +826,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
@@ -868,473 +871,473 @@
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="23" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11">
+      <c r="A6" s="24">
         <v>1</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="6">
+      <c r="C6" s="3"/>
+      <c r="D6" s="15">
         <f>D7+D8+D9+D10+D11+D12+D13+D14</f>
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="A7" s="25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="16">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="A8" s="25">
         <v>1.2</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="16">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="A9" s="25">
         <v>1.3</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="16">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+      <c r="A10" s="25">
         <v>1.4</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="14">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="25">
+        <v>1.6</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="26">
+        <v>1.7</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="22">
-        <v>1.7</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="27">
+        <v>1.8</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="24">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="9">
-        <v>1.8</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="15">
+      <c r="D14" s="18">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12">
+      <c r="A15" s="28">
         <v>2</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="7">
+      <c r="C15" s="14"/>
+      <c r="D15" s="19">
         <f>D16+D17+D18+D19+D20</f>
         <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+      <c r="A16" s="25">
         <v>2.1</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="14">
+      <c r="C16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+      <c r="A17" s="25">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="14">
+      <c r="C17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+      <c r="A18" s="25">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="14">
+      <c r="C18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="22">
+      <c r="A19" s="26">
         <v>2.4</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="24">
+      <c r="C19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="17">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="9">
+      <c r="A20" s="27">
         <v>2.5</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="15">
+      <c r="C20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="18">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12">
+      <c r="A21" s="28">
         <v>3</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="7">
+      <c r="C21" s="14"/>
+      <c r="D21" s="19">
         <f>D22+D23+D24+D25+D26</f>
         <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+      <c r="A22" s="25">
         <v>3.1</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="14">
+      <c r="C22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+      <c r="A23" s="25">
         <v>3.2</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="14">
+      <c r="C23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+      <c r="A24" s="25">
         <v>3.3</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="14">
+      <c r="C24" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+      <c r="A25" s="25">
         <v>3.4</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="24">
+      <c r="C25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="17">
         <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="2">
+      <c r="A26" s="25">
         <v>3.5</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="15">
+      <c r="C26" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="18">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="12">
+      <c r="A27" s="28">
         <v>4</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="7">
+      <c r="C27" s="14"/>
+      <c r="D27" s="19">
         <f>D28+D29+D30+D31+D32</f>
         <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
+      <c r="A28" s="25">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="14">
+      <c r="C28" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
+      <c r="A29" s="25">
         <v>4.2</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="14">
+      <c r="C29" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
+      <c r="A30" s="25">
         <v>4.3</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="14">
+      <c r="C30" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="9">
+      <c r="A31" s="27">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="24">
+      <c r="C31" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="17">
         <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="9">
+      <c r="A32" s="27">
         <v>4.5</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="15">
+      <c r="C32" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="18">
         <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="12">
+      <c r="A33" s="28">
         <v>4</v>
       </c>
       <c r="B33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="7">
+      <c r="C33" s="14"/>
+      <c r="D33" s="19">
         <f>D34+D35+D36+D37+D38</f>
         <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2">
+      <c r="A34" s="25">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="14">
+      <c r="C34" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2">
+      <c r="A35" s="25">
         <v>4.2</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="14">
+      <c r="C35" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2">
+      <c r="A36" s="25">
         <v>4.3</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="14">
+      <c r="C36" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="16">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="9">
+      <c r="A37" s="27">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="24">
+      <c r="C37" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="17">
         <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="9">
+      <c r="A38" s="27">
         <v>4.5</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="15">
+      <c r="C38" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="18">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed duration of hours for gdp -02
</commit_message>
<xml_diff>
--- a/Schedule Management .xlsx
+++ b/Schedule Management .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538360\Documents\github\GDP-1-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320EAF8C-C133-4646-8453-BD19CDA0E8ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE50558A-E3D9-4207-97B4-0CFF3562F34A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,65 +468,65 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -812,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D285C303-1EFA-4ED6-8202-1217355840E9}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -826,13 +826,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -844,8 +844,8 @@
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -857,8 +857,8 @@
         <v>4</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -871,474 +871,474 @@
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="24">
+      <c r="A6" s="22">
         <v>1</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="15">
+      <c r="D6" s="13">
         <f>D7+D8+D9+D10+D11+D12+D13+D14</f>
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="25">
+      <c r="A7" s="23">
         <v>1.1000000000000001</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="14">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25">
+      <c r="A8" s="23">
         <v>1.2</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="14">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="25">
+      <c r="A9" s="23">
         <v>1.3</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="14">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25">
+      <c r="A10" s="23">
         <v>1.4</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="14">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25">
+      <c r="A11" s="23">
         <v>1.5</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="14">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25">
+      <c r="A12" s="23">
         <v>1.6</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="14">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="26">
+      <c r="A13" s="24">
         <v>1.7</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="15">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="27">
+      <c r="A14" s="25">
         <v>1.8</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="16">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="28">
+      <c r="A15" s="26">
         <v>2</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="19">
+      <c r="C15" s="12"/>
+      <c r="D15" s="17">
         <f>D16+D17+D18+D19+D20</f>
         <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="25">
+      <c r="A16" s="23">
         <v>2.1</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="16">
+      <c r="C16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="14">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="25">
+      <c r="A17" s="23">
         <v>2.2000000000000002</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="16">
+      <c r="C17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="14">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="25">
+      <c r="A18" s="23">
         <v>2.2999999999999998</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="16">
+      <c r="C18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="14">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="26">
+      <c r="A19" s="24">
         <v>2.4</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="17">
+      <c r="C19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="15">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="27">
+      <c r="A20" s="25">
         <v>2.5</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="18">
+      <c r="C20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="16">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="28">
+      <c r="A21" s="26">
         <v>3</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="19">
+      <c r="C21" s="12"/>
+      <c r="D21" s="17">
         <f>D22+D23+D24+D25+D26</f>
         <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25">
+      <c r="A22" s="23">
         <v>3.1</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="16">
+      <c r="C22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="14">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="25">
+      <c r="A23" s="23">
         <v>3.2</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="16">
+      <c r="C23" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="14">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="25">
+      <c r="A24" s="23">
         <v>3.3</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="16">
+      <c r="C24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="14">
         <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="25">
+      <c r="A25" s="23">
         <v>3.4</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="17">
+      <c r="C25" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="15">
         <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="25">
+      <c r="A26" s="23">
         <v>3.5</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="18">
+      <c r="C26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="16">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28">
+      <c r="A27" s="26">
         <v>4</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="19">
+      <c r="C27" s="12"/>
+      <c r="D27" s="17">
         <f>D28+D29+D30+D31+D32</f>
         <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="25">
+      <c r="A28" s="23">
         <v>4.0999999999999996</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="16">
+      <c r="C28" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="14">
         <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="25">
+      <c r="A29" s="23">
         <v>4.2</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="16">
+      <c r="C29" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="14">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="25">
+      <c r="A30" s="23">
         <v>4.3</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="16">
+      <c r="C30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="14">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="27">
+      <c r="A31" s="25">
         <v>4.4000000000000004</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="17">
+      <c r="C31" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="15">
         <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="27">
+      <c r="A32" s="25">
         <v>4.5</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="18">
+      <c r="C32" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="16">
         <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="28">
+      <c r="A33" s="26">
         <v>4</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="19">
+      <c r="C33" s="12"/>
+      <c r="D33" s="17">
         <f>D34+D35+D36+D37+D38</f>
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="25">
+      <c r="A34" s="23">
         <v>4.0999999999999996</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="16">
-        <v>35</v>
+      <c r="C34" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="14">
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="25">
+      <c r="A35" s="23">
         <v>4.2</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="16">
-        <v>35</v>
+      <c r="C35" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="14">
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="25">
+      <c r="A36" s="23">
         <v>4.3</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="16">
-        <v>35</v>
+      <c r="C36" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="14">
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="27">
+      <c r="A37" s="25">
         <v>4.4000000000000004</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="17">
-        <v>45</v>
+      <c r="C37" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="15">
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="27">
+      <c r="A38" s="25">
         <v>4.5</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="18">
-        <v>50</v>
+      <c r="C38" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="16">
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated schedule  management in readme file accordingly.
</commit_message>
<xml_diff>
--- a/Schedule Management .xlsx
+++ b/Schedule Management .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538360\Documents\github\GDP-1-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A8EB2D-0DFE-404B-90D9-11AF66F8BBCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5F8712-4930-48E8-B206-271562A8B493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50" yWindow="290" windowWidth="9520" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -812,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D285C303-1EFA-4ED6-8202-1217355840E9}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Made some changes in readme file and corrections in schedule management file
</commit_message>
<xml_diff>
--- a/Schedule Management .xlsx
+++ b/Schedule Management .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538360\Documents\github\GDP-1-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5F8712-4930-48E8-B206-271562A8B493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0F326C-0B2A-45A5-8165-70B55C544057}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50" yWindow="290" windowWidth="9520" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50" yWindow="270" windowWidth="9520" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -812,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D285C303-1EFA-4ED6-8202-1217355840E9}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="33" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>42</v>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="34" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23">
-        <v>4.0999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>33</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="35" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="23">
-        <v>4.2</v>
+        <v>5.2</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>34</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="36" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="23">
-        <v>4.3</v>
+        <v>5.3</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>35</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="37" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="25">
-        <v>4.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>36</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="38" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="25">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>37</v>

</xml_diff>